<commit_message>
Add Report,Metrics,MindMaps etc in desktop app
</commit_message>
<xml_diff>
--- a/Test-Cases/Desktop_App.xlsx
+++ b/Test-Cases/Desktop_App.xlsx
@@ -1,31 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IT Training BD\Class_3_ManualTestCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git Projects\Manual-Testing\Test-Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F48F6833-3692-4352-85B4-1F7EA61EA19A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5E8E766-9D6D-41CC-B2B0-E430314A3787}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Registration" sheetId="1" r:id="rId1"/>
+    <sheet name="Report" sheetId="2" r:id="rId2"/>
+    <sheet name="TestMetrics" sheetId="3" r:id="rId3"/>
+    <sheet name="Mind Maps" sheetId="4" r:id="rId4"/>
+    <sheet name="Bug Report" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="126">
   <si>
     <t>Project Name :</t>
   </si>
@@ -239,29 +251,197 @@
     <t>Verify the registration functionality with valid email address and give numeric password more than 8 characters.</t>
   </si>
   <si>
-    <t>1. Enter invalid email address.
+    <t>Email : mahbubislam@gmail.com
+Password : 123456789</t>
+  </si>
+  <si>
+    <t>Account should not be created successfully and showing "Password must contain at least one upper case character".</t>
+  </si>
+  <si>
+    <t>Account is not being created successfully and showing "Password must contain at least one upper case character".</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>TEST-CASE</t>
+  </si>
+  <si>
+    <t>NOT EXECUTED</t>
+  </si>
+  <si>
+    <t>OUT OF SCOPE</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Test Case Report</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Project Name  - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Module Name  - </t>
+  </si>
+  <si>
+    <t>Test Case Version</t>
+  </si>
+  <si>
+    <t>Written By</t>
+  </si>
+  <si>
+    <t>Reviewed By</t>
+  </si>
+  <si>
+    <t>TEST EXECUTION REPORT</t>
+  </si>
+  <si>
+    <t>Test Case</t>
+  </si>
+  <si>
+    <t>Not Executed</t>
+  </si>
+  <si>
+    <t>Out Of Scope</t>
+  </si>
+  <si>
+    <t>Total TC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grand Total  </t>
+  </si>
+  <si>
+    <t>MAHBUB ISLAM</t>
+  </si>
+  <si>
+    <t>Out of Scope</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total No. </t>
+  </si>
+  <si>
+    <t>Metrics Name</t>
+  </si>
+  <si>
+    <t>Count</t>
+  </si>
+  <si>
+    <t>Total Number of Test Cases</t>
+  </si>
+  <si>
+    <t>Number Of Test Cases Not Executed</t>
+  </si>
+  <si>
+    <t>Number Of Test Cases Executed</t>
+  </si>
+  <si>
+    <t>Number Of Test Cases Passed</t>
+  </si>
+  <si>
+    <t>Number Of Test Cases Failed</t>
+  </si>
+  <si>
+    <t>Test Metrics</t>
+  </si>
+  <si>
+    <t>SL</t>
+  </si>
+  <si>
+    <t>Metrics</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Reesult(%)</t>
+  </si>
+  <si>
+    <t>Percentage Of Test Cases  Executed</t>
+  </si>
+  <si>
+    <t>(Number Of Test Cases Executed/Total Number Of Test Cases)*100</t>
+  </si>
+  <si>
+    <t>Percentage Of Test Cases Not  Executed</t>
+  </si>
+  <si>
+    <t>(Number Of Test Cases Not Executed/Total Number Of Test Cases)*100</t>
+  </si>
+  <si>
+    <t>Percentage Of Test Cases Passed</t>
+  </si>
+  <si>
+    <t>(Number Of Test Cases Passed/Total Number Of Test Cases)*100</t>
+  </si>
+  <si>
+    <t>Percentage Of Test Cases Failed</t>
+  </si>
+  <si>
+    <t>(Number Of Test Cases Failed/Total Number Of Test Cases)*100</t>
+  </si>
+  <si>
+    <t>Bug reporting</t>
+  </si>
+  <si>
+    <t>Issue</t>
+  </si>
+  <si>
+    <t>Verify the registration functionality with valid</t>
+  </si>
+  <si>
+    <t>email address and give numeric password</t>
+  </si>
+  <si>
+    <t>more than 8 characters.</t>
+  </si>
+  <si>
+    <t>Reproducing Steps</t>
+  </si>
+  <si>
+    <t>1. Enter valid email address.
 2. Insert numeric password more than 8 characters .
 3. Click "SIGN UP, IT'S FREE!" button.</t>
   </si>
   <si>
-    <t>Email : mahbubislam@gmail.com
-Password : 123456789</t>
-  </si>
-  <si>
-    <t>Account should not be created successfully and showing "Password must contain at least one upper case character".</t>
-  </si>
-  <si>
-    <t>Account is not being created successfully and showing "Password must contain at least one upper case character".</t>
-  </si>
-  <si>
-    <t>PENDING</t>
+    <t>Enter valid email address.</t>
+  </si>
+  <si>
+    <t>Insert numeric password more than 8 characters.</t>
+  </si>
+  <si>
+    <t>Click "SIGN UP, IT'S FREE!" button</t>
+  </si>
+  <si>
+    <t>Production</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>Severity :</t>
+  </si>
+  <si>
+    <t>Module :</t>
+  </si>
+  <si>
+    <t>ENV :</t>
+  </si>
+  <si>
+    <t>Screenshot :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Responsible QA </t>
+  </si>
+  <si>
+    <t>https://prnt.sc/RbFqexKGwiyC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -277,8 +457,99 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Comfortaa"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF002060"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -291,8 +562,128 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FF00"/>
+        <bgColor rgb="FF00FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2DBDB"/>
+        <bgColor rgb="FFF2DBDB"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB6DDE8"/>
+        <bgColor rgb="FFB6DDE8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA4C2F4"/>
+        <bgColor rgb="FFA4C2F4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9EAD3"/>
+        <bgColor rgb="FFD9EAD3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCFE2F3"/>
+        <bgColor rgb="FFCFE2F3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9900"/>
+        <bgColor rgb="FFFF9900"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD8D8D8"/>
+        <bgColor rgb="FFD8D8D8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -300,12 +691,203 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -322,9 +904,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -336,10 +915,140 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="9" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="12" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="5" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="15" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="16" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="10" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="8" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink 2" xfId="4" xr:uid="{3FB1B97C-C2F1-4D5C-99E9-2F0D63ED2928}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{D795843C-3F61-4D2E-BD38-B170C20F8924}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{8332ADA2-4195-4BDE-9859-9AAFB8652DC9}"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
@@ -393,6 +1102,1164 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:view3D>
+      <c:rotX val="50"/>
+      <c:rotY val="0"/>
+      <c:depthPercent val="100"/>
+      <c:rAngAx val="0"/>
+    </c:view3D>
+    <c:floor>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:floor>
+    <c:sideWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:sideWall>
+    <c:backWall>
+      <c:thickness val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+        <a:sp3d/>
+      </c:spPr>
+    </c:backWall>
+    <c:plotArea>
+      <c:layout/>
+      <c:pie3DChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="20000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:sp3d/>
+            </c:spPr>
+          </c:dPt>
+          <c:dLbls>
+            <c:spPr>
+              <a:pattFill prst="pct75">
+                <a:fgClr>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:fgClr>
+                <a:bgClr>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:bgClr>
+              </a:pattFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:leaderLines>
+              <c:spPr>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="50000"/>
+                      <a:lumOff val="50000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:leaderLines>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Report!$N$9:$N$12</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>PASS</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FAIL</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Not Executed</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Out of Scope</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Report!$O$9:$O$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A180-4D34-8458-E55A6C29E94D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="1"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+      </c:pie3DChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="39000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="accent6">
+        <a:lumMod val="60000"/>
+        <a:lumOff val="40000"/>
+      </a:schemeClr>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="25000"/>
+          <a:lumOff val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="264">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="39000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="pct75">
+        <a:fgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+    <cs:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:effectLst>
+        <a:outerShdw blurRad="254000" sx="102000" sy="102000" algn="ctr" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="20000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+          <a:alpha val="39000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>209550</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15E41AC9-A364-A215-787D-18454EB0FC99}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2BB2CDE-60ED-293C-83ED-D4C1864C2F5A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2438400" y="1143000"/>
+          <a:ext cx="7915275" cy="4362450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF">
+            <a:shade val="85000"/>
+          </a:srgbClr>
+        </a:solidFill>
+        <a:ln w="88900" cap="sq">
+          <a:solidFill>
+            <a:srgbClr val="FFFFFF"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="55000" dist="18000" dir="5400000" algn="tl" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="40000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="twoPt" dir="t">
+            <a:rot lat="0" lon="0" rev="7200000"/>
+          </a:lightRig>
+        </a:scene3d>
+        <a:sp3d>
+          <a:bevelT w="25400" h="19050"/>
+          <a:contourClr>
+            <a:srgbClr val="FFFFFF"/>
+          </a:contourClr>
+        </a:sp3d>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -660,16 +2527,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
     <col min="2" max="2" width="25.5703125" customWidth="1"/>
     <col min="3" max="3" width="15" style="4" customWidth="1"/>
-    <col min="4" max="4" width="31.28515625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="31.28515625" style="8" customWidth="1"/>
     <col min="5" max="5" width="18.140625" customWidth="1"/>
     <col min="6" max="6" width="33.28515625" customWidth="1"/>
     <col min="7" max="7" width="25.5703125" customWidth="1"/>
@@ -681,7 +2548,7 @@
     <col min="14" max="14" width="16.28515625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -691,8 +2558,12 @@
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
       <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G1" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="H1" s="14"/>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -702,8 +2573,15 @@
       <c r="C2" s="2"/>
       <c r="D2" s="3"/>
       <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G2" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="20">
+        <f>COUNTIF(J12:J200,"PASS")</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -713,8 +2591,15 @@
       <c r="C3" s="2"/>
       <c r="D3" s="3"/>
       <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G3" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" s="20">
+        <f>COUNTIF(J12:J200,"FAIL")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -724,8 +2609,15 @@
       <c r="C4" s="2"/>
       <c r="D4" s="3"/>
       <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G4" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" s="20">
+        <f>COUNTIF(J12:J200,"NOT EXECUTED")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -735,8 +2627,15 @@
       <c r="C5" s="2"/>
       <c r="D5" s="3"/>
       <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G5" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="H5" s="20">
+        <f>COUNTIF(J12:J200,"OUT OF SCOPE")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -746,8 +2645,15 @@
       <c r="C6" s="2"/>
       <c r="D6" s="3"/>
       <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G6" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="H6" s="20">
+        <f>SUM(H2:H5)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -758,7 +2664,7 @@
       <c r="D7" s="3"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -767,7 +2673,7 @@
       <c r="D8" s="3"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="11" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" s="4" customFormat="1">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
@@ -811,35 +2717,35 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="11" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+    <row r="12" spans="1:14" s="10" customFormat="1" ht="90">
+      <c r="A12" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="I12" s="10" t="s">
+      <c r="I12" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="J12" s="56" t="s">
         <v>38</v>
       </c>
       <c r="L12" s="4" t="s">
@@ -850,34 +2756,34 @@
       </c>
       <c r="N12" s="4"/>
     </row>
-    <row r="13" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="8" t="s">
+    <row r="13" spans="1:14" ht="60">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="D13" s="9" t="s">
+      <c r="D13" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="I13" s="10" t="s">
+      <c r="I13" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="J13" s="4" t="s">
+      <c r="J13" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="K13" s="11"/>
+      <c r="K13" s="10"/>
       <c r="L13" s="4" t="s">
         <v>9</v>
       </c>
@@ -885,34 +2791,34 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="8" t="s">
+    <row r="14" spans="1:14" ht="60">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="H14" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="I14" s="10" t="s">
+      <c r="I14" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="J14" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="K14" s="11"/>
+      <c r="K14" s="10"/>
       <c r="L14" s="4" t="s">
         <v>9</v>
       </c>
@@ -920,34 +2826,34 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="8" t="s">
+    <row r="15" spans="1:14" ht="60">
+      <c r="A15" s="11"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G15" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="H15" s="10" t="s">
+      <c r="H15" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="I15" s="10" t="s">
+      <c r="I15" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="J15" s="4" t="s">
+      <c r="J15" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="K15" s="11"/>
+      <c r="K15" s="10"/>
       <c r="L15" s="4" t="s">
         <v>9</v>
       </c>
@@ -955,34 +2861,34 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="8" t="s">
+    <row r="16" spans="1:14" ht="75">
+      <c r="A16" s="11"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="9" t="s">
+      <c r="D16" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H16" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="I16" s="10" t="s">
+      <c r="I16" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="J16" s="4" t="s">
+      <c r="J16" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="K16" s="11"/>
+      <c r="K16" s="10"/>
       <c r="L16" s="4" t="s">
         <v>9</v>
       </c>
@@ -990,34 +2896,34 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="8" t="s">
+    <row r="17" spans="1:13" ht="75">
+      <c r="A17" s="11"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="D17" s="9" t="s">
+      <c r="D17" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="G17" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="H17" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="I17" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="I17" s="10" t="s">
+      <c r="J17" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="J17" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="K17" s="11"/>
+      <c r="K17" s="10"/>
       <c r="L17" s="4" t="s">
         <v>9</v>
       </c>
@@ -1026,9 +2932,10 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A12:A17"/>
     <mergeCell ref="B12:B17"/>
+    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <conditionalFormatting sqref="J12:J17">
     <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
@@ -1056,4 +2963,661 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FCF42C5-CA71-42C5-8279-BF88D3077FC1}">
+  <dimension ref="C6:O18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="23" style="32" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" customWidth="1"/>
+    <col min="15" max="15" width="15.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="3:15" ht="15.75" thickBot="1"/>
+    <row r="7" spans="3:15" ht="32.25" thickBot="1">
+      <c r="C7" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="30"/>
+    </row>
+    <row r="8" spans="3:15" ht="15.75" thickBot="1">
+      <c r="C8" s="31" t="s">
+        <v>74</v>
+      </c>
+      <c r="D8" s="22" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="23"/>
+      <c r="N8" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="O8" s="47" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="3:15" ht="15.75" thickBot="1">
+      <c r="C9" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="23"/>
+      <c r="N9" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="O9" s="50">
+        <f>D18</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="3:15" ht="15.75" thickBot="1">
+      <c r="C10" s="31" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="22">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="23"/>
+      <c r="N10" s="48" t="s">
+        <v>68</v>
+      </c>
+      <c r="O10" s="50">
+        <f>E18</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="3:15" ht="15.75" thickBot="1">
+      <c r="C11" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
+      <c r="G11" s="21"/>
+      <c r="H11" s="23"/>
+      <c r="N11" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="O11" s="50">
+        <f>F18</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="3:15" ht="15.75" thickBot="1">
+      <c r="C12" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="22" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="23"/>
+      <c r="N12" s="49" t="s">
+        <v>86</v>
+      </c>
+      <c r="O12" s="50">
+        <f>G18</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="3:15" ht="15.75" thickBot="1">
+      <c r="C13" s="31" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="23"/>
+    </row>
+    <row r="14" spans="3:15">
+      <c r="C14" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="26"/>
+    </row>
+    <row r="15" spans="3:15" ht="15.75" thickBot="1">
+      <c r="C15" s="27"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="23"/>
+    </row>
+    <row r="16" spans="3:15" ht="31.5">
+      <c r="C16" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="34" t="s">
+        <v>68</v>
+      </c>
+      <c r="F16" s="34" t="s">
+        <v>81</v>
+      </c>
+      <c r="G16" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="H16" s="35" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8">
+      <c r="C17" s="45" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="36">
+        <f>Registration!H2</f>
+        <v>5</v>
+      </c>
+      <c r="E17" s="37">
+        <f>Registration!H3</f>
+        <v>1</v>
+      </c>
+      <c r="F17" s="38">
+        <f>Registration!H4</f>
+        <v>0</v>
+      </c>
+      <c r="G17" s="39">
+        <f>Registration!H4</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="40">
+        <f>Registration!H6</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" ht="19.5" thickBot="1">
+      <c r="C18" s="46" t="s">
+        <v>84</v>
+      </c>
+      <c r="D18" s="41">
+        <f>D17</f>
+        <v>5</v>
+      </c>
+      <c r="E18" s="42">
+        <f>E17</f>
+        <v>1</v>
+      </c>
+      <c r="F18" s="41">
+        <f>F17</f>
+        <v>0</v>
+      </c>
+      <c r="G18" s="41">
+        <f>G17</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="43">
+        <f>H17</f>
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="D11:H11"/>
+    <mergeCell ref="D13:H13"/>
+    <mergeCell ref="C14:H15"/>
+    <mergeCell ref="D9:H9"/>
+    <mergeCell ref="D10:H10"/>
+    <mergeCell ref="D12:H12"/>
+    <mergeCell ref="C7:H7"/>
+    <mergeCell ref="D8:H8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{064B6016-355D-44D5-B8D1-584E1555E11C}">
+  <dimension ref="A1:I16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="44.5703125" style="12" customWidth="1"/>
+    <col min="2" max="2" width="27.42578125" style="12" customWidth="1"/>
+    <col min="3" max="3" width="7" customWidth="1"/>
+    <col min="4" max="4" width="7.28515625" customWidth="1"/>
+    <col min="5" max="5" width="8" customWidth="1"/>
+    <col min="6" max="6" width="9.28515625" style="12" customWidth="1"/>
+    <col min="7" max="7" width="36" customWidth="1"/>
+    <col min="8" max="8" width="64.5703125" customWidth="1"/>
+    <col min="9" max="9" width="36.28515625" style="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="51" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="52" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B2" s="12">
+        <f>Report!H18</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="B3" s="12">
+        <f>Report!F18</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" s="12">
+        <f>TestMetrics!B2-TestMetrics!B3</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="12">
+        <f>Report!D18</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B6" s="12">
+        <f>Report!E18</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="21" customHeight="1">
+      <c r="F11" s="53" t="s">
+        <v>95</v>
+      </c>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="53"/>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="F12" s="54" t="s">
+        <v>96</v>
+      </c>
+      <c r="G12" s="55" t="s">
+        <v>97</v>
+      </c>
+      <c r="H12" s="55" t="s">
+        <v>98</v>
+      </c>
+      <c r="I12" s="54" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="F13" s="59">
+        <v>1</v>
+      </c>
+      <c r="G13" s="60" t="s">
+        <v>100</v>
+      </c>
+      <c r="H13" s="60" t="s">
+        <v>101</v>
+      </c>
+      <c r="I13" s="59">
+        <f>(B4/B2)*100</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="F14" s="59">
+        <v>2</v>
+      </c>
+      <c r="G14" s="60" t="s">
+        <v>102</v>
+      </c>
+      <c r="H14" s="60" t="s">
+        <v>103</v>
+      </c>
+      <c r="I14" s="59">
+        <f>(B3/B2)*100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="F15" s="59">
+        <v>3</v>
+      </c>
+      <c r="G15" s="60" t="s">
+        <v>104</v>
+      </c>
+      <c r="H15" s="60" t="s">
+        <v>105</v>
+      </c>
+      <c r="I15" s="59">
+        <f>(B5/B2)*100</f>
+        <v>83.333333333333343</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="F16" s="59">
+        <v>4</v>
+      </c>
+      <c r="G16" s="60" t="s">
+        <v>106</v>
+      </c>
+      <c r="H16" s="60" t="s">
+        <v>107</v>
+      </c>
+      <c r="I16" s="59">
+        <f>(B6/B2)*100</f>
+        <v>16.666666666666664</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="F11:I11"/>
+  </mergeCells>
+  <phoneticPr fontId="14" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0297A259-FCA5-46D3-967E-ABA51A39B27C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S18" sqref="S18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F63211F5-5F39-433D-972C-438630DDB9CF}">
+  <dimension ref="E8:J28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="5" max="5" width="15.5703125" style="63" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="8" spans="5:10">
+      <c r="E8" s="58" t="s">
+        <v>108</v>
+      </c>
+      <c r="F8" s="57"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="57"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="57"/>
+    </row>
+    <row r="9" spans="5:10">
+      <c r="E9" s="57"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="57"/>
+      <c r="H9" s="57"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="57"/>
+    </row>
+    <row r="10" spans="5:10" ht="23.25" customHeight="1">
+      <c r="E10" s="62" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="13"/>
+    </row>
+    <row r="11" spans="5:10" ht="17.25" customHeight="1">
+      <c r="E11" s="62" t="s">
+        <v>109</v>
+      </c>
+      <c r="F11" s="61" t="s">
+        <v>110</v>
+      </c>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+    </row>
+    <row r="12" spans="5:10">
+      <c r="E12" s="62"/>
+      <c r="F12" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="13"/>
+    </row>
+    <row r="13" spans="5:10">
+      <c r="E13" s="62"/>
+      <c r="F13" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+    </row>
+    <row r="14" spans="5:10">
+      <c r="E14" s="62"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="13"/>
+    </row>
+    <row r="15" spans="5:10">
+      <c r="E15" s="62" t="s">
+        <v>113</v>
+      </c>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+    </row>
+    <row r="16" spans="5:10">
+      <c r="E16" s="64">
+        <v>1</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+    </row>
+    <row r="17" spans="5:10">
+      <c r="E17" s="64">
+        <v>2</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+    </row>
+    <row r="18" spans="5:10">
+      <c r="E18" s="64">
+        <v>3</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+    </row>
+    <row r="19" spans="5:10">
+      <c r="E19" s="62"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+    </row>
+    <row r="20" spans="5:10">
+      <c r="E20" s="62" t="s">
+        <v>122</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="G20" s="13"/>
+      <c r="H20" s="13"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="13"/>
+    </row>
+    <row r="21" spans="5:10">
+      <c r="E21" s="62"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+    </row>
+    <row r="22" spans="5:10">
+      <c r="E22" s="62" t="s">
+        <v>121</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="13"/>
+      <c r="H22" s="13"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="13"/>
+    </row>
+    <row r="23" spans="5:10">
+      <c r="E23" s="62"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="13"/>
+      <c r="J23" s="13"/>
+    </row>
+    <row r="24" spans="5:10">
+      <c r="E24" s="62" t="s">
+        <v>120</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="13"/>
+      <c r="J24" s="13"/>
+    </row>
+    <row r="25" spans="5:10">
+      <c r="E25" s="62"/>
+      <c r="F25" s="13"/>
+      <c r="G25" s="13"/>
+      <c r="H25" s="13"/>
+      <c r="I25" s="13"/>
+      <c r="J25" s="13"/>
+    </row>
+    <row r="26" spans="5:10">
+      <c r="E26" s="62" t="s">
+        <v>123</v>
+      </c>
+      <c r="F26" s="65" t="s">
+        <v>125</v>
+      </c>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+    </row>
+    <row r="27" spans="5:10">
+      <c r="E27" s="62"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+    </row>
+    <row r="28" spans="5:10">
+      <c r="E28" s="62" t="s">
+        <v>124</v>
+      </c>
+      <c r="F28" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
+      <c r="I28" s="13"/>
+      <c r="J28" s="13"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E8:J9"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="F26" r:id="rId1" xr:uid="{EDB87D5B-BC46-48FC-AE3C-2CE1D5D66B32}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>